<commit_message>
Zeiterfassung_Welsch_Dennis.xlsx : zeit erfassung ausgefüllt Erfahrungsbericht_Dennis_Welsch.docx : erfahrungsbericht ausgefüllt
</commit_message>
<xml_diff>
--- a/1. Projektplanung und Dokumentation/1.1 Zeiterfassung/Zeiterfassung_Welsch_Dennis.xlsx
+++ b/1. Projektplanung und Dokumentation/1.1 Zeiterfassung/Zeiterfassung_Welsch_Dennis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwels\VSCODE\RaytRazor\1. Projektplanung\1.1 Zeiterfassung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwels\CLionProjects\RaytRazor\1. Projektplanung und Dokumentation\1.1 Zeiterfassung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB6821C-D4A7-494C-90B8-EC34C17C17F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F3B3FE-7109-4920-8749-9718537BB294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{13671DE0-EAD2-44F3-A1E0-C608E2EB2296}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>Name:</t>
   </si>
@@ -95,10 +95,52 @@
     <t>Notfall besprechung</t>
   </si>
   <si>
-    <t>Programmieren</t>
-  </si>
-  <si>
     <t>Erstes konzept der Raytracer Math library</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufgabenverteilung, Organisierung </t>
+  </si>
+  <si>
+    <t>Offline-Treffen</t>
+  </si>
+  <si>
+    <t>Aufgaben</t>
+  </si>
+  <si>
+    <t>Importer anpassungen</t>
+  </si>
+  <si>
+    <t>Importer überarbeiten</t>
+  </si>
+  <si>
+    <t>Licht sphären farbe, Erfahrungsbericht, Präsentation vorbereitung</t>
+  </si>
+  <si>
+    <t>Licht sphären anzeigen</t>
+  </si>
+  <si>
+    <t>Bugfixing und Farbige objekte anzeigen</t>
+  </si>
+  <si>
+    <t>Bugfixing von preview</t>
+  </si>
+  <si>
+    <t>Indices hinzugefügt</t>
+  </si>
+  <si>
+    <t>vertice / indice anpassen</t>
+  </si>
+  <si>
+    <t>bugfixing</t>
+  </si>
+  <si>
+    <t>Implementierung der Preview</t>
+  </si>
+  <si>
+    <t>Converter hinzugefügt</t>
+  </si>
+  <si>
+    <t>Converter angepasst &amp; bugfixing</t>
   </si>
 </sst>
 </file>
@@ -450,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D11EDF1B-A292-464D-9512-73DA35F01323}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -589,26 +631,277 @@
         <v>4</v>
       </c>
       <c r="C12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="6" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>45593</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-    </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
+      <c r="A14" s="4">
+        <v>45598</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
+      <c r="A15" s="4">
+        <v>45600</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2.15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
+      <c r="A16" s="4">
+        <v>45605</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>45612</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>45616</v>
+      </c>
+      <c r="B18" s="2">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>45619</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>45624</v>
+      </c>
+      <c r="B20" s="2">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>45628</v>
+      </c>
+      <c r="B21" s="2">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>45638</v>
+      </c>
+      <c r="B22" s="2">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>45671</v>
+      </c>
+      <c r="B23" s="2">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>45672</v>
+      </c>
+      <c r="B24" s="2">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>45673</v>
+      </c>
+      <c r="B25" s="2">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>45674</v>
+      </c>
+      <c r="B26" s="2">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>45675</v>
+      </c>
+      <c r="B27" s="2">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>45676</v>
+      </c>
+      <c r="B28" s="2">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>45677</v>
+      </c>
+      <c r="B29" s="2">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>45678</v>
+      </c>
+      <c r="B30" s="2">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <v>45679</v>
+      </c>
+      <c r="B31" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -619,18 +912,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -778,18 +1071,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC5825A0-9928-4DC4-96F2-A5F9419A53C9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE7FC1F3-F6F1-4513-BD25-A27348CF4110}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE7FC1F3-F6F1-4513-BD25-A27348CF4110}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC5825A0-9928-4DC4-96F2-A5F9419A53C9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>